<commit_message>
data laden gaat goed
</commit_message>
<xml_diff>
--- a/Group16.xlsx
+++ b/Group16.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjribeiro/Documents/courses/AE4423 Airline Planning &amp; Optimisation/2024/assignments/To Students/Assignment2/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gijsvdklink/Documents/Airline planning and optimisation /AIRLINE_PLANNING2/Assignment-2-Airline-Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34A48920-18D6-AD45-A9F0-DD186E054F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658AF93D-C750-C044-AD19-ECD40E12B5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="4160" windowWidth="26440" windowHeight="15440" xr2:uid="{500A615B-0ADD-F34B-B4C2-C068173D5017}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{500A615B-0ADD-F34B-B4C2-C068173D5017}"/>
   </bookViews>
   <sheets>
     <sheet name="Group 16" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="31">
   <si>
     <t>FNC</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>Day 1</t>
-  </si>
-  <si>
-    <t>Hub</t>
   </si>
 </sst>
 </file>
@@ -533,7 +530,7 @@
   <dimension ref="A2:AG405"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:AG405"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -543,9 +540,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B2" s="5"/>
       <c r="D2" s="4" t="s">
         <v>30</v>
       </c>
@@ -563,9 +558,7 @@
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="B3" s="3"/>
       <c r="D3" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>